<commit_message>
Rev 3: Software Test Completed
</commit_message>
<xml_diff>
--- a/ece3232-software-testdata.xlsx
+++ b/ece3232-software-testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macke\Desktop\School\ECE3232\ECE3232-ServoMotor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5E140BB-C936-4E05-B6A5-A5C378963312}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B167D8BC-030E-4BEA-AFAE-941A1DE7B0AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F224E6A2-BD44-4B3A-9C07-41B3DFE3B2C6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t xml:space="preserve">software testing </t>
   </si>
@@ -128,6 +128,30 @@
   <si>
     <t>KSDK implementation of sprintf 
 doesn’t handle float</t>
+  </si>
+  <si>
+    <t>{1 ,8 ,7 ,5, 4 , 5, 9,14}(uint16_t)</t>
+  </si>
+  <si>
+    <t>SendtoDaq()</t>
+  </si>
+  <si>
+    <t>Putty Output: position to go to decrementing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because we are giving it a constant value
+the error will keep on decrementing 
+to control the motor
+</t>
+  </si>
+  <si>
+    <t>Putty Output: position to go to is: 33000</t>
+  </si>
+  <si>
+    <t>Gather_Data()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Putty Output Showing a binary count going from 000 --&gt; 111 and then reset </t>
   </si>
 </sst>
 </file>
@@ -163,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,6 +203,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -198,8 +228,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{181DD3AA-F2B5-4735-8F8E-EDEC1F4EEC58}" name="Table2" displayName="Table2" ref="A2:G28" totalsRowShown="0">
-  <autoFilter ref="A2:G28" xr:uid="{4821E373-8444-4928-9DB2-1D3A40D198FB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{181DD3AA-F2B5-4735-8F8E-EDEC1F4EEC58}" name="Table2" displayName="Table2" ref="A2:G29" totalsRowShown="0">
+  <autoFilter ref="A2:G29" xr:uid="{4821E373-8444-4928-9DB2-1D3A40D198FB}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{30069FE7-687F-4748-945D-15670072B564}" name="Module "/>
     <tableColumn id="2" xr3:uid="{B77AF6B2-FAE3-4CBE-8462-CBCA17252762}" name="Data"/>
@@ -510,29 +540,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF2E30B-874E-453A-9B97-93877122DE6A}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -693,6 +723,75 @@
       </c>
       <c r="G8" s="5" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>